<commit_message>
Figure edits based on Nick's feedback, plot medians instead of median, use shapes to denote experiment or whether mice cleared by day 7, examine intra- and inter-group variation, update Readme to include new anaylsis script.
</commit_message>
<xml_diff>
--- a/submission/table_S11_family_stats_dn1to0.xlsx
+++ b/submission/table_S11_family_stats_dn1to0.xlsx
@@ -411,10 +411,10 @@
         </is>
       </c>
       <c r="F2">
-        <v>0.2183426581309664</v>
+        <v>0.1565201397829686</v>
       </c>
       <c r="G2">
-        <v>0.01807211044990418</v>
+        <v>0.001103549751701306</v>
       </c>
       <c r="H2">
         <v>4.749745130538936e-08</v>
@@ -443,10 +443,10 @@
         </is>
       </c>
       <c r="F3">
-        <v>0.37054946098121</v>
+        <v>0.4638587456317823</v>
       </c>
       <c r="G3">
-        <v>0.02424249615834159</v>
+        <v>0.0007356998344675372</v>
       </c>
       <c r="H3">
         <v>4.915986210107798e-06</v>
@@ -475,10 +475,10 @@
         </is>
       </c>
       <c r="F4">
-        <v>0.00160192705892125</v>
+        <v>0.001103549751701306</v>
       </c>
       <c r="G4">
-        <v>5.933063181189816e-05</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>1.861878885488437e-05</v>
@@ -507,10 +507,10 @@
         </is>
       </c>
       <c r="F5">
-        <v>0.0008424949717289539</v>
+        <v>0.0003678499172337686</v>
       </c>
       <c r="G5">
-        <v>0.5465656463775683</v>
+        <v>0.6864079455582123</v>
       </c>
       <c r="H5">
         <v>1.861878885488437e-05</v>
@@ -539,10 +539,10 @@
         </is>
       </c>
       <c r="F6">
-        <v>0.05116673687458098</v>
+        <v>0.01839249586168843</v>
       </c>
       <c r="G6">
-        <v>0.0006882353290180187</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>1.861878885488437e-05</v>
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="F7">
-        <v>0.001168813446694394</v>
+        <v>0.0009196247930844216</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -603,10 +603,10 @@
         </is>
       </c>
       <c r="F8">
-        <v>0.02526891608868743</v>
+        <v>0.01710502115137024</v>
       </c>
       <c r="G8">
-        <v>0.000551774875850653</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>2.837858559070229e-05</v>
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="F9">
-        <v>0.004087880531839783</v>
+        <v>0.002207099503402612</v>
       </c>
       <c r="G9">
-        <v>0.000450912801770426</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0.0002042461121129806</v>
@@ -667,10 +667,10 @@
         </is>
       </c>
       <c r="F10">
-        <v>0.0307036019626573</v>
+        <v>0.02335846974434431</v>
       </c>
       <c r="G10">
-        <v>0.007303600776044664</v>
+        <v>0.001471399668935074</v>
       </c>
       <c r="H10">
         <v>0.0002042461121129806</v>
@@ -699,10 +699,10 @@
         </is>
       </c>
       <c r="F11">
-        <v>8.899594771784724e-05</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0.04347155392857779</v>
+        <v>0.0152657715652014</v>
       </c>
       <c r="H11">
         <v>0.00021479552856431</v>
@@ -731,10 +731,10 @@
         </is>
       </c>
       <c r="F12">
-        <v>0.05405613864382042</v>
+        <v>0.04598123965422108</v>
       </c>
       <c r="G12">
-        <v>0.1671403228772983</v>
+        <v>0.1329777450800074</v>
       </c>
       <c r="H12">
         <v>0.0002617144629922837</v>
@@ -763,10 +763,10 @@
         </is>
       </c>
       <c r="F13">
-        <v>0.04274772022047263</v>
+        <v>0.008092698179142909</v>
       </c>
       <c r="G13">
-        <v>4.746450544951853e-05</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0.0003393815576407513</v>
@@ -795,10 +795,10 @@
         </is>
       </c>
       <c r="F14">
-        <v>0.009753955869876058</v>
+        <v>0.004598123965422108</v>
       </c>
       <c r="G14">
-        <v>0.003375912950097005</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0.0009831133037177633</v>
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="F15">
-        <v>0.01820857090307155</v>
+        <v>0.003494574213720802</v>
       </c>
       <c r="G15">
-        <v>0.005600811643043187</v>
+        <v>0.000551774875850653</v>
       </c>
       <c r="H15">
         <v>0.002706450973425734</v>
@@ -859,10 +859,10 @@
         </is>
       </c>
       <c r="F16">
-        <v>0.005909330928465057</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>4.153144226832872e-05</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0.006044335433400369</v>
@@ -891,10 +891,10 @@
         </is>
       </c>
       <c r="F17">
-        <v>0.005339756863070835</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>2.373225272475927e-05</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0.007716848092665235</v>
@@ -923,10 +923,10 @@
         </is>
       </c>
       <c r="F18">
-        <v>0.001423935163485556</v>
+        <v>0.000551774875850653</v>
       </c>
       <c r="G18">
-        <v>0.0003797160435961483</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0.008999256893476004</v>
@@ -955,10 +955,10 @@
         </is>
       </c>
       <c r="F19">
-        <v>0.002248630945670941</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>1.779918954356945e-05</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0.01649781499403696</v>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="F20">
-        <v>0.001263742457593431</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1019,10 +1019,10 @@
         </is>
       </c>
       <c r="F21">
-        <v>0.0003975152331397177</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>1.186612636237963e-05</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <v>0.1885404614229879</v>
@@ -1051,10 +1051,10 @@
         </is>
       </c>
       <c r="F22">
-        <v>0.009623428479889883</v>
+        <v>0.000551774875850653</v>
       </c>
       <c r="G22">
-        <v>0.004242140174550719</v>
+        <v>0</v>
       </c>
       <c r="H22">
         <v>0.2326254804353105</v>
@@ -1083,10 +1083,10 @@
         </is>
       </c>
       <c r="F23">
-        <v>0.001168813446694394</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>0.0001008620740802269</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>0.2326254804353105</v>
@@ -1115,10 +1115,10 @@
         </is>
       </c>
       <c r="F24">
-        <v>0.0003144523486030603</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>0.005772870475297692</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>0.2342572560563358</v>
@@ -1147,10 +1147,10 @@
         </is>
       </c>
       <c r="F25">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>2.373225272475926e-05</v>
+        <v>0</v>
       </c>
       <c r="H25">
         <v>0.629810996203899</v>
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>1.186612636237963e-05</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <v>0.629810996203899</v>
@@ -1211,10 +1211,10 @@
         </is>
       </c>
       <c r="F27">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>1.779918954356945e-05</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>0.629810996203899</v>
@@ -1246,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>1.186612636237963e-05</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <v>0.629810996203899</v>
@@ -1275,7 +1275,7 @@
         </is>
       </c>
       <c r="F29">
-        <v>1.186612636237963e-05</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1307,10 +1307,10 @@
         </is>
       </c>
       <c r="F30">
-        <v>0.122090574142524</v>
+        <v>0.05554533750229906</v>
       </c>
       <c r="G30">
-        <v>0.1587509715390959</v>
+        <v>0.001103549751701306</v>
       </c>
       <c r="H30">
         <v>0.6513531098291647</v>
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="F31">
-        <v>2.966531590594908e-05</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1371,10 +1371,10 @@
         </is>
       </c>
       <c r="F32">
-        <v>1.779918954356945e-05</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>0.0001245943268049862</v>
+        <v>0</v>
       </c>
       <c r="H32">
         <v>0.6736431807094503</v>
@@ -1403,10 +1403,10 @@
         </is>
       </c>
       <c r="F33">
-        <v>0.0004331136122268566</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="H33">
         <v>0.6736431807094503</v>
@@ -1435,10 +1435,10 @@
         </is>
       </c>
       <c r="F34">
-        <v>1.186612636237963e-05</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>2.373225272475926e-05</v>
+        <v>0</v>
       </c>
       <c r="H34">
         <v>0.7480283663619358</v>
@@ -1467,10 +1467,10 @@
         </is>
       </c>
       <c r="F35">
-        <v>0.004467596575435931</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>0.01122535553881113</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <v>0.7570039079323414</v>
@@ -1499,10 +1499,10 @@
         </is>
       </c>
       <c r="F36">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>2.373225272475927e-05</v>
+        <v>0</v>
       </c>
       <c r="H36">
         <v>0.8541970781351468</v>
@@ -1531,10 +1531,10 @@
         </is>
       </c>
       <c r="F37">
-        <v>0.01533103526019449</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>5.933063181189817e-05</v>
+        <v>0</v>
       </c>
       <c r="H37">
         <v>0.9120696870076535</v>
@@ -1566,7 +1566,7 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -1595,10 +1595,10 @@
         </is>
       </c>
       <c r="F39">
-        <v>0.001245943268049861</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>0.001495131921659834</v>
+        <v>0</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -1630,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="G40">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -1659,7 +1659,7 @@
         </is>
       </c>
       <c r="F41">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1691,7 +1691,7 @@
         </is>
       </c>
       <c r="F42">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -1723,7 +1723,7 @@
         </is>
       </c>
       <c r="F43">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -1755,10 +1755,10 @@
         </is>
       </c>
       <c r="F44">
-        <v>1.779918954356945e-05</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>1.186612636237963e-05</v>
+        <v>0</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -1787,7 +1787,7 @@
         </is>
       </c>
       <c r="F45">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -1822,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -1851,7 +1851,7 @@
         </is>
       </c>
       <c r="F47">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -1886,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -1915,7 +1915,7 @@
         </is>
       </c>
       <c r="F49">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -1950,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -1979,10 +1979,10 @@
         </is>
       </c>
       <c r="F51">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G51">
-        <v>1.186612636237963e-05</v>
+        <v>0</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -2011,10 +2011,10 @@
         </is>
       </c>
       <c r="F52">
-        <v>5.933063181189816e-06</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>1.186612636237963e-05</v>
+        <v>0</v>
       </c>
       <c r="H52">
         <v>1</v>

</xml_diff>